<commit_message>
PackageDiagramm aktualisiert nach Umzug zu ArchCNL weitere SPARQL-Queries
</commit_message>
<xml_diff>
--- a/Issue-Tracker.xlsx
+++ b/Issue-Tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\GitHub\Mari-Wie\ArchCnl\ArchCnlDocumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\GitHub\Mari-Wie\ArchCnl-Projekte\ArchCnlDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
   <si>
     <t>Issue</t>
   </si>
@@ -303,9 +303,6 @@
   </si>
   <si>
     <t>ggf. Umbau auf Alternative</t>
-  </si>
-  <si>
-    <t>Christian</t>
   </si>
   <si>
     <t>Iac/Entwicklung im Containter</t>
@@ -684,7 +681,7 @@
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -715,7 +712,7 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s">
         <v>21</v>
@@ -738,7 +735,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
         <v>36</v>
@@ -792,7 +789,7 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -801,7 +798,7 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
         <v>36</v>
@@ -812,7 +809,7 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -821,7 +818,7 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
@@ -841,7 +838,7 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
         <v>36</v>
@@ -864,7 +861,7 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
         <v>36</v>
@@ -883,9 +880,6 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>84</v>
-      </c>
       <c r="G9" t="s">
         <v>24</v>
       </c>
@@ -988,9 +982,6 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
-        <v>84</v>
-      </c>
       <c r="G15" t="s">
         <v>24</v>
       </c>
@@ -1005,9 +996,6 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="E16" t="s">
-        <v>84</v>
-      </c>
       <c r="G16" t="s">
         <v>24</v>
       </c>
@@ -1017,13 +1005,13 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -1034,13 +1022,13 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G18" t="s">
         <v>28</v>
@@ -1051,13 +1039,13 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G19" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Issues zur Initialisierung des Tools ergänzt
</commit_message>
<xml_diff>
--- a/Issue-Tracker.xlsx
+++ b/Issue-Tracker.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\GitHub\Mari-Wie\ArchCnl-Projekte\ArchCnlDocumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\GitHub\Mari-Wie\ArchCNL Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E1843F-6107-48FC-B8A4-2E4B02A26EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28570" windowHeight="13850"/>
+    <workbookView xWindow="10140" yWindow="1590" windowWidth="24750" windowHeight="17770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issue-Tracker" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="110">
   <si>
     <t>Issue</t>
   </si>
@@ -280,9 +281,6 @@
     <t>Java-Module System</t>
   </si>
   <si>
-    <t>Umbau auf Java Module, um Packages zusammenzuführen</t>
-  </si>
-  <si>
     <t>Gradle/Maven Auflösung</t>
   </si>
   <si>
@@ -330,12 +328,68 @@
   </si>
   <si>
     <t>Stardog-Version aktualisieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link mit "sandr" entfernen </t>
+  </si>
+  <si>
+    <t>Für eine der Ontologien wird eine URIverwendet, die eine ausgedachte URL mit "sandr" (für Sandra) verweist. Die URI soll durch eine sinnvolle(z.B. informatik.uni-hamburg.de/…/swk/…) ersetzt werden</t>
+  </si>
+  <si>
+    <t>Es gibt gleich zu Anfang des Durchlaufs einen Performancefresser (ist bei verfolgung der Logs ersichtlich), dieser und weitere sollen analysiert und, wenn möglich, ausgebaut werden.</t>
+  </si>
+  <si>
+    <t>Performanceoptimierung</t>
+  </si>
+  <si>
+    <t>unnötige github-Repositories löschen</t>
+  </si>
+  <si>
+    <t>nicht mehr verwendete Repositories löschen</t>
+  </si>
+  <si>
+    <t>Niklas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updgrade auf Java 13 </t>
+  </si>
+  <si>
+    <t>Upgrade auf die neueste Java-Version</t>
+  </si>
+  <si>
+    <t>sonstiges</t>
+  </si>
+  <si>
+    <t>Umbau auf Java Module, um Packages zusammenzuführen, wenn sinnvoll</t>
+  </si>
+  <si>
+    <t>Logs ergänzen</t>
+  </si>
+  <si>
+    <t>Die bestehenden Logs sollen sukzessive um weitere sinnvolle Logeinträge ergänzt werden.
+Außerdem soll das Log zusätzlich in ein File ermöglicht werden. Das File-Ablage soll über einen relativen Pfad oder Environment Variable erfolgen.</t>
+  </si>
+  <si>
+    <t>Es geht erstmal nur um die Analyse, welche Packages sich gegenseitig aufrufen. In der Architektur war geplant, dass sich die Packages nicht gegnseitig aufrufen mit Außnahme von CNLToolchain und common. 
+Die Aufrufe sollen im Package-Diagramm ergänzt werden und deren Ausbau als Issues mit Prio 1 aufgenommen werden</t>
+  </si>
+  <si>
+    <t>Abhängigkeiten erkennen und dokumentieren</t>
+  </si>
+  <si>
+    <t>Package-Diagramm überprüfen und aktualisieren</t>
+  </si>
+  <si>
+    <t>Whiteboard-Foto als Diagramm</t>
+  </si>
+  <si>
+    <t>einschl. Überprüfung auf Korrektheit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,21 +446,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H1048576" totalsRowShown="0">
-  <autoFilter ref="A1:H1048576"/>
-  <sortState ref="A2:H54">
-    <sortCondition ref="C2:C54"/>
-    <sortCondition ref="A2:A54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:H1048576" totalsRowShown="0">
+  <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H55">
+    <sortCondition ref="C1:C1048576"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Issue-Nr"/>
-    <tableColumn id="2" name="Issue"/>
-    <tableColumn id="8" name="Prio"/>
-    <tableColumn id="3" name="Vorbedingungen"/>
-    <tableColumn id="7" name="Bearbeiter"/>
-    <tableColumn id="4" name="Status"/>
-    <tableColumn id="5" name="MP/BA/MA/DI"/>
-    <tableColumn id="6" name="Erläuterung" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Issue-Nr"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Issue"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Prio"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Vorbedingungen"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Bearbeiter"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="MP/BA/MA/DI"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Erläuterung" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -674,14 +727,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
         <v>21</v>
@@ -735,7 +788,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
         <v>36</v>
@@ -755,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
         <v>36</v>
@@ -775,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
         <v>36</v>
@@ -789,7 +842,7 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -798,7 +851,7 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
         <v>36</v>
@@ -809,7 +862,7 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -818,402 +871,408 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>98</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>36</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>89</v>
+      </c>
       <c r="G16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="E17" t="s">
-        <v>85</v>
+      <c r="D17">
+        <v>46</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
       </c>
+      <c r="H17" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
-        <v>88</v>
-      </c>
       <c r="G18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="E19" t="s">
-        <v>88</v>
-      </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>36</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>11</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>10</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" t="s">
         <v>24</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="G23" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>15</v>
-      </c>
-      <c r="B25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
       </c>
       <c r="G26" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>14</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="G27" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>
@@ -1222,98 +1281,92 @@
         <v>36</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
         <v>27</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C32">
-        <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
         <v>27</v>
@@ -1322,38 +1375,35 @@
         <v>36</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C34">
-        <v>5</v>
-      </c>
-      <c r="E34" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>30</v>
-      </c>
-      <c r="B35" t="s">
-        <v>67</v>
+        <v>14</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E35" t="s">
         <v>27</v>
@@ -1362,178 +1412,301 @@
         <v>36</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C36">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" t="s">
+        <v>27</v>
       </c>
       <c r="G36" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C37">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>27</v>
       </c>
       <c r="G37" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C38">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D38">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C39">
-        <v>9</v>
-      </c>
-      <c r="D39">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G39" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C40">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
       </c>
       <c r="G40" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C41">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
       </c>
       <c r="G41" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>41</v>
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" t="s">
+        <v>36</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>9</v>
+      </c>
+      <c r="G44" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>44</v>
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>9</v>
+      </c>
+      <c r="G45" t="s">
+        <v>46</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46">
+        <v>9</v>
+      </c>
+      <c r="D46">
+        <v>15</v>
+      </c>
+      <c r="G46" t="s">
+        <v>46</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>22</v>
+      </c>
+      <c r="G47" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="B48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48">
+        <v>9</v>
+      </c>
+      <c r="G48" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49">
+        <v>9</v>
+      </c>
+      <c r="G49" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
PackageDiagramm XTEXT korrigiert Issue-Tracker.xlsx
</commit_message>
<xml_diff>
--- a/Issue-Tracker.xlsx
+++ b/Issue-Tracker.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\GitHub\Mari-Wie\ArchCNL Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E1843F-6107-48FC-B8A4-2E4B02A26EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C370124B-E32C-4E9A-A4FD-385C088658C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="1590" windowWidth="24750" windowHeight="17770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issue-Tracker" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="111">
   <si>
     <t>Issue</t>
   </si>
@@ -52,9 +61,6 @@
   </si>
   <si>
     <t>Bearbeiter</t>
-  </si>
-  <si>
-    <t>Dokumentation aufarbeiten</t>
   </si>
   <si>
     <t>XTEND lauffähig</t>
@@ -384,6 +390,12 @@
   </si>
   <si>
     <t>einschl. Überprüfung auf Korrektheit</t>
+  </si>
+  <si>
+    <t>Dokumentation aufarbeiten und ins GitHub Wiki</t>
+  </si>
+  <si>
+    <t>Issues in GitHub-Issues</t>
   </si>
 </sst>
 </file>
@@ -447,8 +459,12 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:H1048576" totalsRowShown="0">
-  <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H55">
+  <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="5">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H54">
     <sortCondition ref="C1:C1048576"/>
   </sortState>
   <tableColumns count="8">
@@ -730,11 +746,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -756,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -765,16 +781,16 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -785,13 +801,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -808,13 +824,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -828,53 +844,53 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -882,24 +898,24 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>95</v>
@@ -908,78 +924,78 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" t="s">
-        <v>94</v>
+        <v>100</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>106</v>
@@ -988,18 +1004,15 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>107</v>
@@ -1008,189 +1021,189 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>101</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>46</v>
-      </c>
-      <c r="G17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>9</v>
-      </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="G18" t="s">
-        <v>25</v>
+      <c r="D18">
+        <v>46</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1198,497 +1211,509 @@
       <c r="G23" t="s">
         <v>24</v>
       </c>
+      <c r="H23" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
-        <v>84</v>
-      </c>
       <c r="G25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G26" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" t="s">
         <v>27</v>
-      </c>
-      <c r="G28" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
-      <c r="D30">
-        <v>10</v>
+      <c r="E30" t="s">
+        <v>26</v>
       </c>
       <c r="G30" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
       <c r="G31" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>15</v>
-      </c>
-      <c r="B33" t="s">
-        <v>31</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>27</v>
       </c>
-      <c r="G33" t="s">
-        <v>36</v>
-      </c>
       <c r="H33" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
       <c r="G34" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>14</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" t="s">
-        <v>36</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>16</v>
-      </c>
-      <c r="B36" t="s">
-        <v>32</v>
+      <c r="B36" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
-      <c r="D36" t="s">
-        <v>34</v>
-      </c>
       <c r="E36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
-      <c r="D37">
-        <v>15</v>
+      <c r="D37" t="s">
+        <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G37" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D38">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
       </c>
       <c r="G38" t="s">
         <v>73</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C39">
         <v>4</v>
       </c>
+      <c r="D39">
+        <v>16</v>
+      </c>
       <c r="G39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="G40" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>24</v>
       </c>
-      <c r="B40" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40">
-        <v>5</v>
-      </c>
-      <c r="E40" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" t="s">
-        <v>36</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>25</v>
-      </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C41">
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C42">
         <v>5</v>
       </c>
       <c r="E42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A43">
         <v>27</v>
       </c>
-      <c r="G42" t="s">
-        <v>36</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>30</v>
-      </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C43">
         <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45">
         <v>19</v>
       </c>
-      <c r="B44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44">
-        <v>9</v>
-      </c>
-      <c r="G44" t="s">
-        <v>25</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>20</v>
-      </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C45">
         <v>9</v>
       </c>
       <c r="G45" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C46">
         <v>9</v>
       </c>
-      <c r="D46">
-        <v>15</v>
-      </c>
       <c r="G46" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C47">
         <v>9</v>
       </c>
       <c r="D47">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C48">
         <v>9</v>
       </c>
+      <c r="D48">
+        <v>22</v>
+      </c>
       <c r="G48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C49">
         <v>9</v>
       </c>
       <c r="G49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H49" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>29</v>
+      </c>
+      <c r="B50" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>49</v>
+      <c r="C50">
+        <v>9</v>
+      </c>
+      <c r="G50" t="s">
+        <v>27</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>